<commit_message>
calculating slope of curve vs distance upchannel
</commit_message>
<xml_diff>
--- a/data/bedthickness_vs_slope_and_rsquared.xlsx
+++ b/data/bedthickness_vs_slope_and_rsquared.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\HS_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17909FE-D2CB-4016-849E-FFD1901BA7F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9344B834-CE76-4DBA-B532-8511982BF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{43419ABB-FFCE-4E4C-BB56-74F822066E51}"/>
+    <workbookView xWindow="-23148" yWindow="-576" windowWidth="23256" windowHeight="12456" xr2:uid="{43419ABB-FFCE-4E4C-BB56-74F822066E51}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -17442,24 +17442,24 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" customWidth="1"/>
-    <col min="11" max="11" width="34.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" customWidth="1"/>
+    <col min="11" max="11" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17503,7 +17503,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -17547,7 +17547,7 @@
         <v>117.71</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -17591,7 +17591,7 @@
         <v>477.81</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -17635,7 +17635,7 @@
         <v>320.58</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -17679,7 +17679,7 @@
         <v>145.88</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -17723,7 +17723,7 @@
         <v>142.13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -17767,7 +17767,7 @@
         <v>322.27999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -17811,7 +17811,7 @@
         <v>360.56</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -17828,7 +17828,7 @@
         <v>124.9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -17845,7 +17845,7 @@
         <v>273.08</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
@@ -17862,7 +17862,7 @@
         <v>399.22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>493.23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
@@ -17896,7 +17896,7 @@
         <v>440.79</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
@@ -17913,7 +17913,7 @@
         <v>481.75</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
@@ -17930,7 +17930,7 @@
         <v>564.28</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
@@ -17947,7 +17947,7 @@
         <v>376.08</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
@@ -17964,7 +17964,7 @@
         <v>221.75</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
@@ -17981,7 +17981,7 @@
         <v>141.33000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -17998,7 +17998,7 @@
         <v>82.53</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -18015,7 +18015,7 @@
         <v>342.86</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -18032,7 +18032,7 @@
         <v>345.95</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>289.67</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -18066,7 +18066,7 @@
         <v>211.86</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -18083,7 +18083,7 @@
         <v>226.67</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -18100,7 +18100,7 @@
         <v>178.84</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>129.76</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -18134,7 +18134,7 @@
         <v>166.11</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -18162,7 +18162,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18177,7 +18177,7 @@
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bunch a new stuff
</commit_message>
<xml_diff>
--- a/data/bedthickness_vs_slope_and_rsquared.xlsx
+++ b/data/bedthickness_vs_slope_and_rsquared.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sam\Documents\HS_project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9344B834-CE76-4DBA-B532-8511982BF194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FDE5C0-7A1E-4BBE-A986-51FE8D5181B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-576" windowWidth="23256" windowHeight="12456" xr2:uid="{43419ABB-FFCE-4E4C-BB56-74F822066E51}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{43419ABB-FFCE-4E4C-BB56-74F822066E51}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -251,6 +251,422 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(data!$L$2:$L$5,data!$L$11:$L$20)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>585.23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1311.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1810.08</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>157.27000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2171.6799999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1967.81</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1661.42</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1486.61</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1181.31</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1001.58</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>780.02</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>452.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>291.85000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>35.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(data!$G$2:$G$5,data!$G$11:$G$20)</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>-1.2200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>-1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>-1E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>-1.1999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>-1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>-1E-4</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>5.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>2.9999999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>-4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>-1E-4</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>-4.0000000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>5.9999999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>-1.2999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6455-446C-A299-A3028094A884}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="166480031"/>
+        <c:axId val="61623359"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="166480031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61623359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="61623359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="166480031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -271,7 +687,532 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>slope</a:t>
+              <a:t>stdev of beds</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs r^2</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.10537270341207348"/>
+                  <c:y val="-0.23044692330125402"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$B$2:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.46470420699623521</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.053451272405769</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.3761055372559987</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.70339478333086</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6089717684021529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4355638300589537</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.4093015182106237</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$F$2:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>0.67559999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0000000000000002E-6</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>5.6500000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>0.253</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>0.50190000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>0.12609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>0.36609999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0D9C-41DB-9C7E-2C1B1E6C11C7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="620519472"/>
+        <c:axId val="620517392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="620519472"/>
+        <c:scaling>
+          <c:logBase val="10"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Bed Thickness (m)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620517392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="620517392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>R Squared</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t>  of Curvature-Distance Function</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620519472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>correl</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
@@ -320,7 +1261,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -351,7 +1292,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="log"/>
+            <c:trendlineType val="linear"/>
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
@@ -423,30 +1364,30 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>data!$G$2:$G$8</c:f>
+              <c:f>data!$I$2:$I$8</c:f>
               <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>-1.2200000000000001E-2</c:v>
+                <c:pt idx="0">
+                  <c:v>-0.82193054839658275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.0000000000000002E-5</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>-1.6999999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>-1E-3</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>-8.8999999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>2.3E-3</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>-2.0999999999999999E-3</c:v>
+                  <c:v>-2.3569658651410269E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-0.237688558995372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.15892415822066094</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.70844188639698968</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.60504212789059564</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.35505270693792934</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -454,7 +1395,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7F09-4181-B089-A30DBE7CC9D8}"/>
+              <c16:uniqueId val="{00000001-C1E1-4C71-9B8D-B8B20BFC9AC7}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -645,7 +1586,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1054,7 +1995,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1579,7 +2520,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2104,7 +3045,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2510,7 +3451,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2908,7 +3849,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3433,7 +4374,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3981,6 +4922,876 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="2"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="5.5736644872510857E-2"/>
+                  <c:y val="0.28758662008244268"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>(data!$L$6:$L$8,data!$L$23:$L$32)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>1320.88</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1847.91</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1629.22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1891.78</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1773.06</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1688.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1532.72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1381.16</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1212.1300000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1072.92</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>874.94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>739.11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>570.28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>(data!$G$6:$G$8,data!$G$23:$G$32)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>-8.8999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-2.0999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.2999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-5.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.1000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1.9E-3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-2.5000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.2999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.9E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5000000000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0419-4047-AE47-5A99941727F8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="166480031"/>
+        <c:axId val="61623359"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="166480031"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61623359"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="61623359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="166480031"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>slope</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs avg thick</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-5.6360673665791776E-2"/>
+                  <c:y val="0.19392935258092739"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>data!$C$2:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3443750000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3766666666666669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3691666666666666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2358333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.708947368421053</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.9133333333333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>data!$G$2:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>-1.2200000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-2.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>-1.6999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>-1E-3</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>-8.8999999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>2.3E-3</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>-2.0999999999999999E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7F09-4181-B089-A30DBE7CC9D8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="620519472"/>
+        <c:axId val="620517392"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="620519472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620517392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="620517392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="620519472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -4491,7 +6302,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4900,7 +6711,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5273,7 +7084,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5798,7 +7609,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6171,7 +7982,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -6607,940 +8418,6 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="620519472"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>stdev of beds</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs r^2</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="log"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="0.10537270341207348"/>
-                  <c:y val="-0.23044692330125402"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>data!$B$2:$B$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.46470420699623521</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.053451272405769</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.3761055372559987</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.70339478333086</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6089717684021529</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.4355638300589537</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.4093015182106237</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data!$F$2:$F$8</c:f>
-              <c:numCache>
-                <c:formatCode>0.00E+00</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0.67559999999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.0000000000000002E-6</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>5.6500000000000002E-2</c:v>
-                </c:pt>
-                <c:pt idx="3" formatCode="General">
-                  <c:v>0.253</c:v>
-                </c:pt>
-                <c:pt idx="4" formatCode="General">
-                  <c:v>0.50190000000000001</c:v>
-                </c:pt>
-                <c:pt idx="5" formatCode="General">
-                  <c:v>0.12609999999999999</c:v>
-                </c:pt>
-                <c:pt idx="6" formatCode="General">
-                  <c:v>0.36609999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-0D9C-41DB-9C7E-2C1B1E6C11C7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="620519472"/>
-        <c:axId val="620517392"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="620519472"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Bed Thickness (m)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="620517392"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="620517392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>R Squared</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>  of Curvature-Distance Function</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="620519472"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>correl</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs avg thick</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-5.6360673665791776E-2"/>
-                  <c:y val="0.19392935258092739"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>data!$C$2:$C$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>0.995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3443750000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.3766666666666669</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3691666666666666</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2358333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.708947368421053</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.9133333333333331</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>data!$I$2:$I$8</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>-0.82193054839658275</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-2.3569658651410269E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-0.237688558995372</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-0.15892415822066094</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-0.70844188639698968</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-0.60504212789059564</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.35505270693792934</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-C1E1-4C71-9B8D-B8B20BFC9AC7}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="620519472"/>
-        <c:axId val="620517392"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="620519472"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="620517392"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="620517392"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -7950,6 +8827,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors18.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -12398,7 +13355,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -12914,7 +13871,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style18.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13430,7 +14387,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -13946,7 +14903,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14462,7 +15419,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -14978,7 +15935,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -15494,7 +16451,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16010,7 +16967,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -16526,7 +17483,1118 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>120311</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>113979</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>26375</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>152616</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F37AB76A-C567-D32C-3D6E-AF3D59F539F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>891540</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>2157774</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>15777</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCC23F5C-3EB3-4349-A6E3-4571FE1C4AED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -17438,28 +19506,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B4C629D-1284-4F44-A136-6BBB39DD89B5}">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A7" sqref="A7"/>
+      <selection pane="topRight" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" customWidth="1"/>
+    <col min="11" max="11" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17503,7 +19574,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -17547,7 +19618,7 @@
         <v>117.71</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -17591,7 +19662,7 @@
         <v>477.81</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -17635,7 +19706,7 @@
         <v>320.58</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -17679,7 +19750,7 @@
         <v>145.88</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -17723,7 +19794,7 @@
         <v>142.13</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -17767,7 +19838,7 @@
         <v>322.27999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -17811,10 +19882,19 @@
         <v>360.56</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="F11">
+        <v>0.72699999999999998</v>
+      </c>
+      <c r="G11">
+        <v>-1.1999999999999999E-3</v>
+      </c>
+      <c r="H11">
+        <v>0.19370000000000001</v>
+      </c>
       <c r="K11">
         <v>1390.61</v>
       </c>
@@ -17828,10 +19908,19 @@
         <v>124.9</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
+      <c r="F12">
+        <v>0.55679999999999996</v>
+      </c>
+      <c r="G12">
+        <v>-1.5E-3</v>
+      </c>
+      <c r="H12">
+        <v>0.16930000000000001</v>
+      </c>
       <c r="K12">
         <v>1440.99</v>
       </c>
@@ -17845,10 +19934,19 @@
         <v>273.08</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>19</v>
       </c>
+      <c r="F13">
+        <v>1.32E-2</v>
+      </c>
+      <c r="G13">
+        <v>-1E-4</v>
+      </c>
+      <c r="H13">
+        <v>-1.66E-2</v>
+      </c>
       <c r="K13">
         <v>1509.91</v>
       </c>
@@ -17862,10 +19960,19 @@
         <v>399.22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="F14">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="G14">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="H14">
+        <v>-3.9800000000000002E-2</v>
+      </c>
       <c r="K14">
         <v>1544.59</v>
       </c>
@@ -17879,10 +19986,19 @@
         <v>493.23</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>21</v>
       </c>
+      <c r="F15">
+        <v>0.28339999999999999</v>
+      </c>
+      <c r="G15">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H15">
+        <v>-0.12709999999999999</v>
+      </c>
       <c r="K15">
         <v>1561.42</v>
       </c>
@@ -17896,10 +20012,19 @@
         <v>440.79</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="F16">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G16">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="H16">
+        <v>7.0099999999999996E-2</v>
+      </c>
       <c r="K16">
         <v>1564.69</v>
       </c>
@@ -17913,10 +20038,19 @@
         <v>481.75</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="F17">
+        <v>9.6199999999999994E-2</v>
+      </c>
+      <c r="G17">
+        <v>-1E-4</v>
+      </c>
+      <c r="H17">
+        <v>8.8999999999999999E-3</v>
+      </c>
       <c r="K17">
         <v>1580.75</v>
       </c>
@@ -17930,10 +20064,19 @@
         <v>564.28</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="F18">
+        <v>0.12429999999999999</v>
+      </c>
+      <c r="G18">
+        <v>-4.0000000000000002E-4</v>
+      </c>
+      <c r="H18">
+        <v>3.5400000000000001E-2</v>
+      </c>
       <c r="K18">
         <v>1597.44</v>
       </c>
@@ -17947,10 +20090,19 @@
         <v>376.08</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="F19">
+        <v>0.1119</v>
+      </c>
+      <c r="G19">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="H19">
+        <v>-0.1648</v>
+      </c>
       <c r="K19">
         <v>1613.88</v>
       </c>
@@ -17964,10 +20116,19 @@
         <v>221.75</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="F20">
+        <v>-1.2999999999999999E-3</v>
+      </c>
+      <c r="G20">
+        <v>-1.2999999999999999E-3</v>
+      </c>
+      <c r="H20">
+        <v>-8.2699999999999996E-2</v>
+      </c>
       <c r="K20">
         <v>1641.14</v>
       </c>
@@ -17981,10 +20142,19 @@
         <v>141.33000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="F23">
+        <v>0.52</v>
+      </c>
+      <c r="G23">
+        <v>-1.2999999999999999E-3</v>
+      </c>
+      <c r="H23">
+        <v>9.35E-2</v>
+      </c>
       <c r="K23">
         <v>1525.3</v>
       </c>
@@ -17998,10 +20168,19 @@
         <v>82.53</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="F24">
+        <v>0.30109999999999998</v>
+      </c>
+      <c r="G24">
+        <v>-5.0000000000000001E-4</v>
+      </c>
+      <c r="H24">
+        <v>4.4999999999999997E-3</v>
+      </c>
       <c r="K24">
         <v>1533.83</v>
       </c>
@@ -18015,10 +20194,19 @@
         <v>342.86</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="F25">
+        <v>0.41239999999999999</v>
+      </c>
+      <c r="G25">
+        <v>-1.1000000000000001E-3</v>
+      </c>
+      <c r="H25">
+        <v>0.1363</v>
+      </c>
       <c r="K25">
         <v>1539.59</v>
       </c>
@@ -18032,10 +20220,19 @@
         <v>345.95</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="F26">
+        <v>0.50139999999999996</v>
+      </c>
+      <c r="G26">
+        <v>-1.9E-3</v>
+      </c>
+      <c r="H26">
+        <v>0.1978</v>
+      </c>
       <c r="K26">
         <v>1558.05</v>
       </c>
@@ -18049,10 +20246,19 @@
         <v>289.67</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
+      <c r="F27">
+        <v>0.15720000000000001</v>
+      </c>
+      <c r="G27">
+        <v>-2.5000000000000001E-3</v>
+      </c>
+      <c r="H27">
+        <v>0.17130000000000001</v>
+      </c>
       <c r="K27">
         <v>1574.22</v>
       </c>
@@ -18066,10 +20272,19 @@
         <v>211.86</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="F28">
+        <v>0.30309999999999998</v>
+      </c>
+      <c r="G28">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="H28">
+        <v>0.34420000000000001</v>
+      </c>
       <c r="K28">
         <v>1604.56</v>
       </c>
@@ -18083,10 +20298,19 @@
         <v>226.67</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
+      <c r="F29">
+        <v>3.5000000000000001E-3</v>
+      </c>
+      <c r="G29">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="H29">
+        <v>-0.15509999999999999</v>
+      </c>
       <c r="K29">
         <v>1622.86</v>
       </c>
@@ -18100,10 +20324,19 @@
         <v>178.84</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="F30">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="G30">
+        <v>1.2999999999999999E-3</v>
+      </c>
+      <c r="H30">
+        <v>-0.32740000000000002</v>
+      </c>
       <c r="K30">
         <v>1641.24</v>
       </c>
@@ -18117,10 +20350,19 @@
         <v>129.76</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
+      <c r="F31">
+        <v>0.74039999999999995</v>
+      </c>
+      <c r="G31">
+        <v>1.9E-3</v>
+      </c>
+      <c r="H31">
+        <v>0.30549999999999999</v>
+      </c>
       <c r="K31">
         <v>1651.17</v>
       </c>
@@ -18134,9 +20376,18 @@
         <v>166.11</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>36</v>
+      </c>
+      <c r="F32">
+        <v>0.78320000000000001</v>
+      </c>
+      <c r="G32">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="H32">
+        <v>-0.34</v>
       </c>
       <c r="K32">
         <v>1661.24</v>
@@ -18153,6 +20404,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -18160,9 +20412,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{080A05F6-290A-483C-848F-D36423700C5E}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A22" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -18177,7 +20429,7 @@
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>